<commit_message>
Checklist_shopping cart and payment Demowebshop.pdf
</commit_message>
<xml_diff>
--- a/Check list Guru99.com.xlsx
+++ b/Check list Guru99.com.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8206d4f600c34161/Рабочий стол/скрины QA/HWs/Checklists/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_F2FC3AEAB9E28401005113B4C48B18E258F8B90C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8790535-63DA-4B05-B2A0-372A9D95091F}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Лист1" sheetId="1" r:id="rId4"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -52,26 +61,26 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">The button (tab) </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Home</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> is active after click</t>
     </r>
@@ -79,26 +88,26 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">The button (tab) </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">Add Customer </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>is active after click</t>
     </r>
@@ -106,26 +115,26 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">The button (tab) </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">Add Tariff Plan </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>is active after click</t>
     </r>
@@ -133,26 +142,26 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>The button (tab)</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> Add Tariff Plan to Customer</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> is active after click</t>
     </r>
@@ -160,26 +169,26 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">The button (tab)  </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Pay Billing</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> is active after click</t>
     </r>
@@ -187,43 +196,43 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">The button (tab)  </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">Delete Customer </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>exist</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>in the Hamburger menu</t>
     </r>
@@ -234,18 +243,18 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Сlose Hamburger menu via</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> Х</t>
     </r>
@@ -259,26 +268,26 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">The logo </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">Guru99 telecom </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>is in the header</t>
     </r>
@@ -286,18 +295,18 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">The main page refreshes after clicking on the logo </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Guru99 telecom</t>
     </r>
@@ -314,26 +323,26 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">Redirect on the page </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Add Customer</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> after click</t>
     </r>
@@ -341,26 +350,26 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">Redirect on the page  </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Add Tariff Plan</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> after click</t>
     </r>
@@ -368,43 +377,43 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">Redirect on the page  </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Add Tariff Plan</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> to Customer </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>after click</t>
     </r>
@@ -412,26 +421,26 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">Redirect on the page  </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Pay Billing</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> after click</t>
     </r>
@@ -439,43 +448,43 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">The button </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">Delete Customer </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>exists</t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>in the main page</t>
     </r>
@@ -483,18 +492,18 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t xml:space="preserve">Return to the main page after clicking on the logo </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
       </rPr>
       <t>Guru99 telecom</t>
     </r>
@@ -503,43 +512,46 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd.mm.yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -549,7 +561,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -582,126 +594,82 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
-    <border/>
+  <borders count="2">
     <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="6" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="6" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -891,309 +859,316 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.13"/>
-    <col customWidth="1" min="2" max="2" width="77.5"/>
-    <col customWidth="1" min="3" max="3" width="37.88"/>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="2" max="2" width="77.44140625" customWidth="1"/>
+    <col min="3" max="3" width="37.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3">
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6">
-        <v>44867.0</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4">
+      <c r="B3" s="5">
+        <v>44867</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7">
-      <c r="A7" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B7" s="11" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="B8" s="11" t="s">
+      <c r="C7" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>2</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="C8" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>3</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="10">
-        <v>4.0</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="C9" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>4</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="C10" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>5</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="B12" s="11" t="s">
+      <c r="C11" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>6</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="10">
-        <v>7.0</v>
-      </c>
-      <c r="B13" s="11" t="s">
+      <c r="C12" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>7</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="10">
-        <v>8.0</v>
-      </c>
-      <c r="B14" s="11" t="s">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>8</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="10">
-        <v>9.0</v>
-      </c>
-      <c r="B15" s="11" t="s">
+      <c r="C14" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>9</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="8" t="s">
+      <c r="C15" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="9"/>
+      <c r="B16" s="3"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17">
-      <c r="A17" s="10">
-        <v>10.0</v>
-      </c>
-      <c r="B17" s="11" t="s">
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>10</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="B18" s="11" t="s">
+      <c r="C17" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>11</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="8" t="s">
+      <c r="C18" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="9"/>
+      <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20">
-      <c r="A20" s="10">
-        <v>12.0</v>
-      </c>
-      <c r="B20" s="15" t="s">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>12</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="8" t="s">
+      <c r="C20" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="9"/>
+      <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22">
-      <c r="A22" s="10">
-        <v>13.0</v>
-      </c>
-      <c r="B22" s="11" t="s">
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
+        <v>13</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="10">
-        <v>14.0</v>
-      </c>
-      <c r="B23" s="11" t="s">
+      <c r="C22" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <v>14</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="10">
-        <v>15.0</v>
-      </c>
-      <c r="B24" s="11" t="s">
+      <c r="C23" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
+        <v>15</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="10">
-        <v>16.0</v>
-      </c>
-      <c r="B25" s="11" t="s">
+      <c r="C24" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
+        <v>16</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="10">
-        <v>17.0</v>
-      </c>
-      <c r="B26" s="11" t="s">
+      <c r="C25" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
+        <v>17</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="10">
-        <v>18.0</v>
-      </c>
-      <c r="B27" s="11" t="s">
+    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
+        <v>18</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="10" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A21:C21"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B1"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="65" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>